<commit_message>
[repo] revisión codigo inflacion 01
</commit_message>
<xml_diff>
--- a/01_datos_crudos/01_03_inpc_concepto_ponds.xlsx
+++ b/01_datos_crudos/01_03_inpc_concepto_ponds.xlsx
@@ -1,80 +1,111 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgejuvenalcamposferreira/Documents/GitHub/mcv_inflacion/01_datos_crudos/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614C94AA-9590-2440-A013-BD6357202AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="24920" yWindow="6620" windowWidth="13840" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t xml:space="preserve">concepto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ponderador_inpc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subyacente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suby_mercancias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suby_merc_alimentos_bebidas_y_tabaco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suby_merc_mercancias_no_alimenticias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suby_servicios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suby_serv_educacion_colegiaturas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suby_serv_vivienda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suby_serv_otros_servicios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no_subyacente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no_suby_agropecuarios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no_suby_frutas_y_verduras</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no_suby_pecuarios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no_suby_energeticos_y_tarifas_autorizadas_por_el_gobierno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no_suby_energeticos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no_suby_tarifas_autorizadas_por_el_gobierno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">canasta_básica</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>concepto</t>
+  </si>
+  <si>
+    <t>ponderador_inpc</t>
+  </si>
+  <si>
+    <t>subyacente</t>
+  </si>
+  <si>
+    <t>suby_mercancias</t>
+  </si>
+  <si>
+    <t>suby_merc_alimentos_bebidas_y_tabaco</t>
+  </si>
+  <si>
+    <t>suby_merc_mercancias_no_alimenticias</t>
+  </si>
+  <si>
+    <t>suby_servicios</t>
+  </si>
+  <si>
+    <t>suby_serv_educacion_colegiaturas</t>
+  </si>
+  <si>
+    <t>suby_serv_vivienda</t>
+  </si>
+  <si>
+    <t>suby_serv_otros_servicios</t>
+  </si>
+  <si>
+    <t>no_subyacente</t>
+  </si>
+  <si>
+    <t>no_suby_agropecuarios</t>
+  </si>
+  <si>
+    <t>no_suby_frutas_y_verduras</t>
+  </si>
+  <si>
+    <t>no_suby_pecuarios</t>
+  </si>
+  <si>
+    <t>no_suby_energeticos_y_tarifas_autorizadas_por_el_gobierno</t>
+  </si>
+  <si>
+    <t>no_suby_energeticos</t>
+  </si>
+  <si>
+    <t>no_suby_tarifas_autorizadas_por_el_gobierno</t>
+  </si>
+  <si>
+    <t>canasta_básica</t>
+  </si>
+  <si>
+    <t>ponderador_inpc_viejo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -102,13 +133,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -390,151 +431,209 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.5" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="n">
-        <v>75.5543393973203</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="B2">
+        <v>75.554339397320305</v>
+      </c>
+      <c r="C2">
+        <v>76.741538251125988</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="n">
-        <v>39.2247730060957</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="B3">
+        <v>39.224773006095702</v>
+      </c>
+      <c r="C3">
+        <v>37.533791983220659</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>20.0737352467231</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="C4">
+        <v>17.214790670186918</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="n">
-        <v>19.1510377593726</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="B5">
+        <v>19.151037759372599</v>
+      </c>
+      <c r="C5">
+        <v>20.319001313033741</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="n">
-        <v>36.3295663912246</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="B6">
+        <v>36.329566391224603</v>
+      </c>
+      <c r="C6">
+        <v>39.207746267905328</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="n">
-        <v>3.60725921697121</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="B7">
+        <v>3.6072592169712099</v>
+      </c>
+      <c r="C7">
+        <v>2.5206846289470755</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="n">
-        <v>15.5066212183997</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="B8">
+        <v>15.506621218399699</v>
+      </c>
+      <c r="C8">
+        <v>18.054989723963121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="n">
-        <v>17.2156859558537</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="B9">
+        <v>17.215685955853701</v>
+      </c>
+      <c r="C9">
+        <v>18.63207191499513</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="n">
-        <v>24.4456606026797</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="B10">
+        <v>24.445660602679698</v>
+      </c>
+      <c r="C10">
+        <v>23.258461748873991</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>10.2171011415222</v>
       </c>
-    </row>
-    <row r="12">
+      <c r="C11">
+        <v>10.657683224792716</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>4.57943855715257</v>
       </c>
-    </row>
-    <row r="13">
+      <c r="C12">
+        <v>4.7788933447153124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="n">
-        <v>5.63766258436963</v>
-      </c>
-    </row>
-    <row r="14">
+      <c r="B13">
+        <v>5.6376625843696297</v>
+      </c>
+      <c r="C13">
+        <v>5.8787898800774032</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>14.2285594611575</v>
       </c>
-    </row>
-    <row r="15">
+      <c r="C14">
+        <v>12.600778524081274</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B15" t="n">
-        <v>9.96504036889179</v>
-      </c>
-    </row>
-    <row r="16">
+      <c r="B15">
+        <v>9.9650403688917901</v>
+      </c>
+      <c r="C15">
+        <v>8.0458008326753649</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="B16" t="n">
-        <v>4.2635190922657</v>
-      </c>
-    </row>
-    <row r="17">
+      <c r="B16">
+        <v>4.2635190922656996</v>
+      </c>
+      <c r="C16">
+        <v>4.5549776914059086</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>36.0538522745195</v>
+      </c>
+      <c r="C17">
+        <v>33.342198150273404</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>